<commit_message>
Completed Microsoft Excel HLOOKUP() Function
</commit_message>
<xml_diff>
--- a/25 - Lookup Functions/Excel103-AdvancedExercises.xlsx
+++ b/25 - Lookup Functions/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/25 - Lookup Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1509" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2776ED47-379D-40FA-9B0A-6FCC2831F4EC}"/>
+  <xr:revisionPtr revIDLastSave="1512" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{325B5CF4-C667-4472-8D9A-26D795661208}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -1966,13 +1966,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3012,10 +3012,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="E2" s="130" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="132"/>
+      <c r="F2" s="130"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -3024,11 +3024,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="130" t="str">
+      <c r="E3" s="131" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="131"/>
+      <c r="F3" s="132"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -3037,8 +3037,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="130"/>
-      <c r="F4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="132"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -3047,8 +3047,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="130"/>
-      <c r="F5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="132"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -3057,8 +3057,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="130"/>
-      <c r="F6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="132"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -3067,8 +3067,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="130"/>
-      <c r="F7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="132"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -3077,8 +3077,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="130"/>
-      <c r="F8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="132"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -3087,8 +3087,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="131"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="132"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -3097,8 +3097,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="130"/>
-      <c r="F10" s="131"/>
+      <c r="E10" s="131"/>
+      <c r="F10" s="132"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -3107,8 +3107,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="130"/>
-      <c r="F11" s="131"/>
+      <c r="E11" s="131"/>
+      <c r="F11" s="132"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -3117,8 +3117,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="130"/>
-      <c r="F12" s="131"/>
+      <c r="E12" s="131"/>
+      <c r="F12" s="132"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -3127,8 +3127,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="130"/>
-      <c r="F13" s="131"/>
+      <c r="E13" s="131"/>
+      <c r="F13" s="132"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -3137,8 +3137,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="130"/>
-      <c r="F14" s="131"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="132"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -3147,8 +3147,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="130"/>
-      <c r="F15" s="131"/>
+      <c r="E15" s="131"/>
+      <c r="F15" s="132"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -3157,8 +3157,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="130"/>
-      <c r="F16" s="131"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="132"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -3167,8 +3167,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="130"/>
-      <c r="F17" s="131"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="132"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -3177,11 +3177,18 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="130"/>
-      <c r="F18" s="131"/>
+      <c r="E18" s="131"/>
+      <c r="F18" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3192,13 +3199,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11502,8 +11502,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="B1:G18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -13019,8 +13019,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
@@ -13067,13 +13067,19 @@
       <c r="A6" s="61" t="s">
         <v>228</v>
       </c>
-      <c r="B6" s="56"/>
+      <c r="B6" s="56">
+        <f>HLOOKUP($B$3,'Master Inventory List'!$A$2:$G$5,3,FALSE)</f>
+        <v>110</v>
+      </c>
     </row>
     <row r="7" spans="1:2" ht="13.5" thickBot="1">
       <c r="A7" s="62" t="s">
         <v>227</v>
       </c>
-      <c r="B7" s="56"/>
+      <c r="B7" s="56">
+        <f>HLOOKUP($B$3,'Master Inventory List'!$A$2:$G$5,4,FALSE)</f>
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -13090,7 +13096,7 @@
   <dimension ref="A2:G5"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>

</xml_diff>

<commit_message>
Completed Microsoft Excel INDEX() Function
</commit_message>
<xml_diff>
--- a/25 - Lookup Functions/Excel103-AdvancedExercises.xlsx
+++ b/25 - Lookup Functions/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/25 - Lookup Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1512" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{325B5CF4-C667-4472-8D9A-26D795661208}"/>
+  <xr:revisionPtr revIDLastSave="1517" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2052432-C0D8-4229-8C3B-20F3266735E8}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -11503,7 +11503,7 @@
   <dimension ref="B1:G18"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -13019,8 +13019,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
@@ -13207,8 +13207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A99380-3415-42C6-8C41-613698A280FA}">
   <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -13247,7 +13247,10 @@
       <c r="B4" s="67">
         <v>1054</v>
       </c>
-      <c r="C4" s="67"/>
+      <c r="C4" s="67" t="str">
+        <f>INDEX('INDEX MATCH Master Emp List'!$A$1:$I$38,10,3)</f>
+        <v>Linda</v>
+      </c>
       <c r="D4" s="67"/>
       <c r="F4" s="68"/>
     </row>
@@ -13255,7 +13258,10 @@
       <c r="B5" s="67">
         <v>1078</v>
       </c>
-      <c r="C5" s="67"/>
+      <c r="C5" s="67" t="str">
+        <f>INDEX('INDEX MATCH Master Emp List'!$A$1:$I$38,4,4)</f>
+        <v>AT</v>
+      </c>
       <c r="D5" s="67"/>
       <c r="F5" s="68"/>
     </row>
@@ -13351,8 +13357,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Completed Microsoft Excel MATCH() Function
</commit_message>
<xml_diff>
--- a/25 - Lookup Functions/Excel103-AdvancedExercises.xlsx
+++ b/25 - Lookup Functions/Excel103-AdvancedExercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/25 - Lookup Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1517" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2052432-C0D8-4229-8C3B-20F3266735E8}"/>
+  <xr:revisionPtr revIDLastSave="1519" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1A5A238-6959-4B0D-85AC-4CCF9D10C976}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1966,13 +1966,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3012,10 +3012,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="130" t="s">
+      <c r="E2" s="132" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="130"/>
+      <c r="F2" s="132"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -3024,11 +3024,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="131" t="str">
+      <c r="E3" s="130" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="132"/>
+      <c r="F3" s="131"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -3037,8 +3037,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="131"/>
-      <c r="F4" s="132"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="131"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -3047,8 +3047,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="131"/>
-      <c r="F5" s="132"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="131"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -3057,8 +3057,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="131"/>
-      <c r="F6" s="132"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="131"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -3067,8 +3067,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="131"/>
-      <c r="F7" s="132"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="131"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -3077,8 +3077,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="131"/>
-      <c r="F8" s="132"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="131"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -3087,8 +3087,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="131"/>
-      <c r="F9" s="132"/>
+      <c r="E9" s="130"/>
+      <c r="F9" s="131"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -3097,8 +3097,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="131"/>
-      <c r="F10" s="132"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="131"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -3107,8 +3107,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="131"/>
-      <c r="F11" s="132"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="131"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -3117,8 +3117,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="131"/>
-      <c r="F12" s="132"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="131"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -3127,8 +3127,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="131"/>
-      <c r="F13" s="132"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="131"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -3137,8 +3137,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="131"/>
-      <c r="F14" s="132"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="131"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -3147,8 +3147,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="131"/>
-      <c r="F15" s="132"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="131"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -3157,8 +3157,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="131"/>
-      <c r="F16" s="132"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="131"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -3167,8 +3167,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="131"/>
-      <c r="F17" s="132"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="131"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -3177,18 +3177,11 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="131"/>
-      <c r="F18" s="132"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3199,6 +3192,13 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13208,7 +13208,7 @@
   <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -13251,7 +13251,10 @@
         <f>INDEX('INDEX MATCH Master Emp List'!$A$1:$I$38,10,3)</f>
         <v>Linda</v>
       </c>
-      <c r="D4" s="67"/>
+      <c r="D4" s="67">
+        <f>MATCH(B4,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
+        <v>1</v>
+      </c>
       <c r="F4" s="68"/>
     </row>
     <row r="5" spans="2:6">
@@ -13262,7 +13265,10 @@
         <f>INDEX('INDEX MATCH Master Emp List'!$A$1:$I$38,4,4)</f>
         <v>AT</v>
       </c>
-      <c r="D5" s="67"/>
+      <c r="D5" s="67">
+        <f>MATCH(B5,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
+        <v>5</v>
+      </c>
       <c r="F5" s="68"/>
     </row>
     <row r="6" spans="2:6">
@@ -13270,7 +13276,10 @@
         <v>1284</v>
       </c>
       <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
+      <c r="D6" s="67">
+        <f>MATCH(B6,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
+        <v>8</v>
+      </c>
       <c r="F6" s="68"/>
     </row>
     <row r="7" spans="2:6">
@@ -13278,7 +13287,10 @@
         <v>1299</v>
       </c>
       <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
+      <c r="D7" s="67">
+        <f>MATCH(B7,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
+        <v>11</v>
+      </c>
       <c r="F7" s="68"/>
     </row>
     <row r="8" spans="2:6">
@@ -13286,7 +13298,10 @@
         <v>1329</v>
       </c>
       <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
+      <c r="D8" s="67">
+        <f>MATCH(B8,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
+        <v>14</v>
+      </c>
       <c r="F8" s="68"/>
     </row>
     <row r="9" spans="2:6">
@@ -13294,7 +13309,10 @@
         <v>1509</v>
       </c>
       <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
+      <c r="D9" s="67">
+        <f>MATCH(B9,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
+        <v>17</v>
+      </c>
       <c r="F9" s="68"/>
     </row>
     <row r="10" spans="2:6">
@@ -13357,7 +13375,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView topLeftCell="B25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Completed Microsoft Excel INDEX() and MATCH() Function Combined
</commit_message>
<xml_diff>
--- a/25 - Lookup Functions/Excel103-AdvancedExercises.xlsx
+++ b/25 - Lookup Functions/Excel103-AdvancedExercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/25 - Lookup Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1519" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1A5A238-6959-4B0D-85AC-4CCF9D10C976}"/>
+  <xr:revisionPtr revIDLastSave="1522" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{473E6E2D-9141-4AA8-A1A9-FD46E73B74CF}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1966,13 +1966,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3012,10 +3012,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="E2" s="130" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="132"/>
+      <c r="F2" s="130"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -3024,11 +3024,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="130" t="str">
+      <c r="E3" s="131" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="131"/>
+      <c r="F3" s="132"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -3037,8 +3037,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="130"/>
-      <c r="F4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="132"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -3047,8 +3047,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="130"/>
-      <c r="F5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="132"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -3057,8 +3057,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="130"/>
-      <c r="F6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="132"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -3067,8 +3067,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="130"/>
-      <c r="F7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="132"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -3077,8 +3077,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="130"/>
-      <c r="F8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="132"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -3087,8 +3087,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="131"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="132"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -3097,8 +3097,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="130"/>
-      <c r="F10" s="131"/>
+      <c r="E10" s="131"/>
+      <c r="F10" s="132"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -3107,8 +3107,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="130"/>
-      <c r="F11" s="131"/>
+      <c r="E11" s="131"/>
+      <c r="F11" s="132"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -3117,8 +3117,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="130"/>
-      <c r="F12" s="131"/>
+      <c r="E12" s="131"/>
+      <c r="F12" s="132"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -3127,8 +3127,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="130"/>
-      <c r="F13" s="131"/>
+      <c r="E13" s="131"/>
+      <c r="F13" s="132"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -3137,8 +3137,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="130"/>
-      <c r="F14" s="131"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="132"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -3147,8 +3147,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="130"/>
-      <c r="F15" s="131"/>
+      <c r="E15" s="131"/>
+      <c r="F15" s="132"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -3157,8 +3157,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="130"/>
-      <c r="F16" s="131"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="132"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -3167,8 +3167,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="130"/>
-      <c r="F17" s="131"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="132"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -3177,11 +3177,18 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="130"/>
-      <c r="F18" s="131"/>
+      <c r="E18" s="131"/>
+      <c r="F18" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3192,13 +3199,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13208,7 +13208,7 @@
   <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -13255,7 +13255,10 @@
         <f>MATCH(B4,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
         <v>1</v>
       </c>
-      <c r="F4" s="68"/>
+      <c r="F4" s="68" t="str">
+        <f>INDEX('INDEX MATCH Master Emp List'!$C$1:$C$38,MATCH(B4,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
+        <v>Howard</v>
+      </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="67">
@@ -13269,7 +13272,10 @@
         <f>MATCH(B5,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
         <v>5</v>
       </c>
-      <c r="F5" s="68"/>
+      <c r="F5" s="68" t="str">
+        <f>INDEX('INDEX MATCH Master Emp List'!$C$1:$C$38,MATCH(B5,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
+        <v>Kendrick</v>
+      </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="67">
@@ -13280,7 +13286,10 @@
         <f>MATCH(B6,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
         <v>8</v>
       </c>
-      <c r="F6" s="68"/>
+      <c r="F6" s="68" t="str">
+        <f>INDEX('INDEX MATCH Master Emp List'!$C$1:$C$38,MATCH(B6,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
+        <v>Frank</v>
+      </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="67">
@@ -13291,7 +13300,10 @@
         <f>MATCH(B7,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
         <v>11</v>
       </c>
-      <c r="F7" s="68"/>
+      <c r="F7" s="68" t="str">
+        <f>INDEX('INDEX MATCH Master Emp List'!$C$1:$C$38,MATCH(B7,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
+        <v>Sandrae</v>
+      </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="67">
@@ -13302,7 +13314,10 @@
         <f>MATCH(B8,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
         <v>14</v>
       </c>
-      <c r="F8" s="68"/>
+      <c r="F8" s="68" t="str">
+        <f>INDEX('INDEX MATCH Master Emp List'!$C$1:$C$38,MATCH(B8,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
+        <v>Tuome</v>
+      </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="67">
@@ -13313,7 +13328,10 @@
         <f>MATCH(B9,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
         <v>17</v>
       </c>
-      <c r="F9" s="68"/>
+      <c r="F9" s="68" t="str">
+        <f>INDEX('INDEX MATCH Master Emp List'!$C$1:$C$38,MATCH(B9,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
+        <v>Pam</v>
+      </c>
     </row>
     <row r="10" spans="2:6">
       <c r="C10" s="67"/>
@@ -13376,7 +13394,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Completed Microsoft Excel INDEX() and MATCH() Function Combined Continued
</commit_message>
<xml_diff>
--- a/25 - Lookup Functions/Excel103-AdvancedExercises.xlsx
+++ b/25 - Lookup Functions/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/25 - Lookup Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1522" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{473E6E2D-9141-4AA8-A1A9-FD46E73B74CF}"/>
+  <xr:revisionPtr revIDLastSave="1528" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{098BF6BF-C4AD-4715-AFE8-2D5B161880B1}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -20,83 +20,84 @@
     <sheet name="HLOOKUP Function" sheetId="22" r:id="rId5"/>
     <sheet name="Master Inventory List" sheetId="23" r:id="rId6"/>
     <sheet name="INDEX MATCH Functions" sheetId="34" r:id="rId7"/>
-    <sheet name="INDEX MATCH Master Emp List" sheetId="5" r:id="rId8"/>
-    <sheet name="LEFT RIGHT MID Functions" sheetId="21" r:id="rId9"/>
-    <sheet name="SEARCH Function" sheetId="24" r:id="rId10"/>
-    <sheet name="CONCATENATE" sheetId="20" r:id="rId11"/>
-    <sheet name="Formula Auditing" sheetId="25" r:id="rId12"/>
-    <sheet name="Watch Window" sheetId="27" r:id="rId13"/>
-    <sheet name="Worksheet Protection" sheetId="26" r:id="rId14"/>
-    <sheet name="Goal Seek" sheetId="31" r:id="rId15"/>
-    <sheet name="Solver" sheetId="30" r:id="rId16"/>
-    <sheet name="Data Table" sheetId="28" r:id="rId17"/>
-    <sheet name="Scenarios" sheetId="29" r:id="rId18"/>
-    <sheet name="Macro" sheetId="32" r:id="rId19"/>
-    <sheet name="Test Macro" sheetId="33" r:id="rId20"/>
+    <sheet name="INDEX MATCH Functions 2" sheetId="36" r:id="rId8"/>
+    <sheet name="INDEX MATCH Master Emp List" sheetId="5" r:id="rId9"/>
+    <sheet name="LEFT RIGHT MID Functions" sheetId="21" r:id="rId10"/>
+    <sheet name="SEARCH Function" sheetId="24" r:id="rId11"/>
+    <sheet name="CONCATENATE" sheetId="20" r:id="rId12"/>
+    <sheet name="Formula Auditing" sheetId="25" r:id="rId13"/>
+    <sheet name="Watch Window" sheetId="27" r:id="rId14"/>
+    <sheet name="Worksheet Protection" sheetId="26" r:id="rId15"/>
+    <sheet name="Goal Seek" sheetId="31" r:id="rId16"/>
+    <sheet name="Solver" sheetId="30" r:id="rId17"/>
+    <sheet name="Data Table" sheetId="28" r:id="rId18"/>
+    <sheet name="Scenarios" sheetId="29" r:id="rId19"/>
+    <sheet name="Macro" sheetId="32" r:id="rId20"/>
+    <sheet name="Test Macro" sheetId="33" r:id="rId21"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'INDEX MATCH Master Emp List'!$A$1:$I$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'INDEX MATCH Master Emp List'!$A$1:$I$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Master Emp List'!$B$1:$I$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SUMIF Function'!$A$2:$E$272</definedName>
     <definedName name="Monthly_Goal">'IF Function'!$I$2</definedName>
-    <definedName name="solver_cvg" localSheetId="15" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="15" hidden="1">1</definedName>
+    <definedName name="solver_cvg" localSheetId="16" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="16" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="15" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="15" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="15" hidden="1">100</definedName>
-    <definedName name="solver_lhs1" localSheetId="15" hidden="1">Solver!$B$8:$E$8</definedName>
-    <definedName name="solver_lhs2" localSheetId="15" hidden="1">Solver!$B$8:$E$8</definedName>
-    <definedName name="solver_lhs3" localSheetId="15" hidden="1">Solver!$B$8:$E$8</definedName>
-    <definedName name="solver_lhs4" localSheetId="15" hidden="1">Solver!$B$8:$E$8</definedName>
-    <definedName name="solver_lhs5" localSheetId="15" hidden="1">Solver!$B$8:$E$8</definedName>
-    <definedName name="solver_lhs6" localSheetId="15" hidden="1">Solver!$E$8</definedName>
-    <definedName name="solver_lhs7" localSheetId="15" hidden="1">Solver!$E$8</definedName>
-    <definedName name="solver_lhs8" localSheetId="15" hidden="1">Solver!$E$8</definedName>
-    <definedName name="solver_lin" localSheetId="15" hidden="1">0</definedName>
-    <definedName name="solver_mip" localSheetId="15" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="15" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="15" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="15" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="16" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="16" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="16" hidden="1">100</definedName>
+    <definedName name="solver_lhs1" localSheetId="16" hidden="1">Solver!$B$8:$E$8</definedName>
+    <definedName name="solver_lhs2" localSheetId="16" hidden="1">Solver!$B$8:$E$8</definedName>
+    <definedName name="solver_lhs3" localSheetId="16" hidden="1">Solver!$B$8:$E$8</definedName>
+    <definedName name="solver_lhs4" localSheetId="16" hidden="1">Solver!$B$8:$E$8</definedName>
+    <definedName name="solver_lhs5" localSheetId="16" hidden="1">Solver!$B$8:$E$8</definedName>
+    <definedName name="solver_lhs6" localSheetId="16" hidden="1">Solver!$E$8</definedName>
+    <definedName name="solver_lhs7" localSheetId="16" hidden="1">Solver!$E$8</definedName>
+    <definedName name="solver_lhs8" localSheetId="16" hidden="1">Solver!$E$8</definedName>
+    <definedName name="solver_lin" localSheetId="16" hidden="1">0</definedName>
+    <definedName name="solver_mip" localSheetId="16" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="16" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="16" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="16" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="15" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="15" hidden="1">2147483647</definedName>
+    <definedName name="solver_neg" localSheetId="16" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="16" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="15" hidden="1">0</definedName>
-    <definedName name="solver_nwt" localSheetId="15" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="16" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="16" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'IF Function'!$I$2</definedName>
-    <definedName name="solver_opt" localSheetId="15" hidden="1">Solver!$H$8</definedName>
-    <definedName name="solver_pre" localSheetId="15" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="15" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="15" hidden="1">2</definedName>
-    <definedName name="solver_rel2" localSheetId="15" hidden="1">2</definedName>
-    <definedName name="solver_rel3" localSheetId="15" hidden="1">2</definedName>
-    <definedName name="solver_rel4" localSheetId="15" hidden="1">2</definedName>
-    <definedName name="solver_rel5" localSheetId="15" hidden="1">2</definedName>
-    <definedName name="solver_rel6" localSheetId="15" hidden="1">2</definedName>
-    <definedName name="solver_rel7" localSheetId="15" hidden="1">2</definedName>
-    <definedName name="solver_rel8" localSheetId="15" hidden="1">2</definedName>
-    <definedName name="solver_rhs1" localSheetId="15" hidden="1">Solver!$B$10:$E$10</definedName>
-    <definedName name="solver_rhs2" localSheetId="15" hidden="1">Solver!$B$10:$E$10</definedName>
-    <definedName name="solver_rhs3" localSheetId="15" hidden="1">Solver!$B$10:$E$10</definedName>
-    <definedName name="solver_rhs4" localSheetId="15" hidden="1">Solver!$B$10:$E$10</definedName>
-    <definedName name="solver_rhs5" localSheetId="15" hidden="1">Solver!$B$10:$E$10</definedName>
-    <definedName name="solver_rhs6" localSheetId="15" hidden="1">Solver!$E$10</definedName>
-    <definedName name="solver_rhs7" localSheetId="15" hidden="1">Solver!$E$10</definedName>
-    <definedName name="solver_rhs8" localSheetId="15" hidden="1">Solver!$E$10</definedName>
-    <definedName name="solver_rlx" localSheetId="15" hidden="1">1</definedName>
-    <definedName name="solver_rsd" localSheetId="15" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="15" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="15" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="15" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="15" hidden="1">100</definedName>
-    <definedName name="solver_tol" localSheetId="15" hidden="1">0.05</definedName>
+    <definedName name="solver_opt" localSheetId="16" hidden="1">Solver!$H$8</definedName>
+    <definedName name="solver_pre" localSheetId="16" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="16" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="16" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="16" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="16" hidden="1">2</definedName>
+    <definedName name="solver_rel4" localSheetId="16" hidden="1">2</definedName>
+    <definedName name="solver_rel5" localSheetId="16" hidden="1">2</definedName>
+    <definedName name="solver_rel6" localSheetId="16" hidden="1">2</definedName>
+    <definedName name="solver_rel7" localSheetId="16" hidden="1">2</definedName>
+    <definedName name="solver_rel8" localSheetId="16" hidden="1">2</definedName>
+    <definedName name="solver_rhs1" localSheetId="16" hidden="1">Solver!$B$10:$E$10</definedName>
+    <definedName name="solver_rhs2" localSheetId="16" hidden="1">Solver!$B$10:$E$10</definedName>
+    <definedName name="solver_rhs3" localSheetId="16" hidden="1">Solver!$B$10:$E$10</definedName>
+    <definedName name="solver_rhs4" localSheetId="16" hidden="1">Solver!$B$10:$E$10</definedName>
+    <definedName name="solver_rhs5" localSheetId="16" hidden="1">Solver!$B$10:$E$10</definedName>
+    <definedName name="solver_rhs6" localSheetId="16" hidden="1">Solver!$E$10</definedName>
+    <definedName name="solver_rhs7" localSheetId="16" hidden="1">Solver!$E$10</definedName>
+    <definedName name="solver_rhs8" localSheetId="16" hidden="1">Solver!$E$10</definedName>
+    <definedName name="solver_rlx" localSheetId="16" hidden="1">1</definedName>
+    <definedName name="solver_rsd" localSheetId="16" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="16" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="16" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="16" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="16" hidden="1">100</definedName>
+    <definedName name="solver_tol" localSheetId="16" hidden="1">0.05</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="15" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="16" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="15" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="16" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="15" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="16" hidden="1">3</definedName>
     <definedName name="Totals">'IF Function'!$F$5:$F$9</definedName>
     <definedName name="Week_1">'IF Function'!$B$5:$B$9</definedName>
     <definedName name="Week_2">'IF Function'!$C$5:$C$9</definedName>
@@ -118,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="284">
   <si>
     <t>Monthly Goal:</t>
   </si>
@@ -1966,13 +1967,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2931,6 +2932,427 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A2:H26"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" customWidth="1"/>
+    <col min="4" max="4" width="3.1796875" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="13">
+      <c r="A2" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" s="39"/>
+      <c r="E2" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>220</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="13">
+      <c r="A3" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="24">
+        <v>13.65</v>
+      </c>
+      <c r="D3" s="37"/>
+      <c r="E3" s="17" t="str">
+        <f>LEFT(A3,3)</f>
+        <v>ACM</v>
+      </c>
+      <c r="F3" s="17" t="str">
+        <f>MID(A3,4,3)</f>
+        <v>110</v>
+      </c>
+      <c r="G3" s="17" t="str">
+        <f>RIGHT(A3,2)</f>
+        <v>WW</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="13">
+      <c r="A4" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="24">
+        <v>12.19</v>
+      </c>
+      <c r="D4" s="37"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="1:8" ht="13">
+      <c r="A5" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="24">
+        <v>10.89</v>
+      </c>
+      <c r="D5" s="37"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="1:8" ht="13">
+      <c r="A6" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" s="24">
+        <v>9.75</v>
+      </c>
+      <c r="D6" s="37"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="1:8" ht="13">
+      <c r="A7" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="24">
+        <v>9.59</v>
+      </c>
+      <c r="D7" s="37"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="1:8" ht="13">
+      <c r="A8" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" s="24">
+        <v>10.4</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:8" ht="13">
+      <c r="A9" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="24">
+        <v>10.56</v>
+      </c>
+      <c r="D9" s="37"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:8" ht="13">
+      <c r="A10" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="24">
+        <v>9.75</v>
+      </c>
+      <c r="D10" s="37"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:8" ht="13">
+      <c r="A11" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" s="24">
+        <v>9.75</v>
+      </c>
+      <c r="D11" s="37"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="1:8" ht="13">
+      <c r="A12" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="C12" s="24">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="D12" s="37"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="1:8" ht="13">
+      <c r="A13" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="24">
+        <v>5.04</v>
+      </c>
+      <c r="D13" s="37"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:8" ht="13">
+      <c r="A14" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14" s="24">
+        <v>3.9</v>
+      </c>
+      <c r="D14" s="37"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:8" ht="13">
+      <c r="A15" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" s="24">
+        <v>4.55</v>
+      </c>
+      <c r="D15" s="37"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:8" ht="13">
+      <c r="A16" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="24">
+        <v>5.2</v>
+      </c>
+      <c r="D16" s="37"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="1:7" ht="13">
+      <c r="A17" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C17" s="24">
+        <v>7.31</v>
+      </c>
+      <c r="D17" s="37"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:7" ht="13">
+      <c r="A18" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="24">
+        <v>6.5</v>
+      </c>
+      <c r="D18" s="37"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="1:7" ht="13">
+      <c r="A19" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="C19" s="24">
+        <v>4.55</v>
+      </c>
+      <c r="D19" s="37"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="1:7" ht="13">
+      <c r="A20" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="C20" s="24">
+        <v>14.3</v>
+      </c>
+      <c r="D20" s="37"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+    </row>
+    <row r="21" spans="1:7" ht="13">
+      <c r="A21" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="C21" s="24">
+        <v>13.81</v>
+      </c>
+      <c r="D21" s="37"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="1:7" ht="13">
+      <c r="A22" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="C22" s="24">
+        <v>7.31</v>
+      </c>
+      <c r="D22" s="37"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+    </row>
+    <row r="23" spans="1:7" ht="13">
+      <c r="A23" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="C23" s="24">
+        <v>7.31</v>
+      </c>
+      <c r="D23" s="37"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+    </row>
+    <row r="24" spans="1:7" ht="13">
+      <c r="A24" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="C24" s="24">
+        <v>7.31</v>
+      </c>
+      <c r="D24" s="37"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="1:7" ht="13">
+      <c r="A25" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="C25" s="24">
+        <v>7.64</v>
+      </c>
+      <c r="D25" s="37"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="1:7" ht="13">
+      <c r="A26" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="C26" s="24">
+        <v>6.14</v>
+      </c>
+      <c r="D26" s="37"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C6"/>
@@ -2988,7 +3410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:F18"/>
@@ -3012,10 +3434,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="130" t="s">
+      <c r="E2" s="132" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="130"/>
+      <c r="F2" s="132"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -3024,11 +3446,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="131" t="str">
+      <c r="E3" s="130" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="132"/>
+      <c r="F3" s="131"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -3037,8 +3459,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="131"/>
-      <c r="F4" s="132"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="131"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -3047,8 +3469,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="131"/>
-      <c r="F5" s="132"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="131"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -3057,8 +3479,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="131"/>
-      <c r="F6" s="132"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="131"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -3067,8 +3489,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="131"/>
-      <c r="F7" s="132"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="131"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -3077,8 +3499,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="131"/>
-      <c r="F8" s="132"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="131"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -3087,8 +3509,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="131"/>
-      <c r="F9" s="132"/>
+      <c r="E9" s="130"/>
+      <c r="F9" s="131"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -3097,8 +3519,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="131"/>
-      <c r="F10" s="132"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="131"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -3107,8 +3529,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="131"/>
-      <c r="F11" s="132"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="131"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -3117,8 +3539,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="131"/>
-      <c r="F12" s="132"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="131"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -3127,8 +3549,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="131"/>
-      <c r="F13" s="132"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="131"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -3137,8 +3559,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="131"/>
-      <c r="F14" s="132"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="131"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -3147,8 +3569,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="131"/>
-      <c r="F15" s="132"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="131"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -3157,8 +3579,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="131"/>
-      <c r="F16" s="132"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="131"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -3167,8 +3589,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="131"/>
-      <c r="F17" s="132"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="131"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -3177,18 +3599,11 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="131"/>
-      <c r="F18" s="132"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3199,6 +3614,13 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3206,7 +3628,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:I14"/>
@@ -3479,7 +3901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:B2"/>
@@ -3508,7 +3930,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:I14"/>
@@ -3782,7 +4204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:D4"/>
@@ -3836,7 +4258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:H11"/>
@@ -4044,7 +4466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="B2:C14"/>
@@ -4151,7 +4573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="B2:G14"/>
@@ -4359,1100 +4781,6 @@
     <oddHeader>&amp;A</oddHeader>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr codeName="Sheet17"/>
-  <dimension ref="A1:I37"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
-  <cols>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7265625" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" style="117" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="115"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="7">
-        <v>1054</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="7">
-        <v>148</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="116">
-        <v>33344</v>
-      </c>
-      <c r="I1" s="115">
-        <v>11.25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="7">
-        <v>1056</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="7">
-        <v>121</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="116">
-        <v>29153</v>
-      </c>
-      <c r="I2" s="115">
-        <v>12.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="7">
-        <v>1067</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="7">
-        <v>123</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="116">
-        <v>32040</v>
-      </c>
-      <c r="I3" s="115">
-        <v>14.55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="7">
-        <v>1075</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="7">
-        <v>126</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="116">
-        <v>33823</v>
-      </c>
-      <c r="I4" s="115">
-        <v>11.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="7">
-        <v>1078</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="7">
-        <v>101</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="116">
-        <v>31503</v>
-      </c>
-      <c r="I5" s="115">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="7">
-        <v>1152</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="7">
-        <v>118</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="116">
-        <v>32894</v>
-      </c>
-      <c r="I6" s="115">
-        <v>12.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="7">
-        <v>1196</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="7">
-        <v>289</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="116">
-        <v>35886</v>
-      </c>
-      <c r="I7" s="115">
-        <v>9.9499999999999993</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="7">
-        <v>1284</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="7">
-        <v>124</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="116">
-        <v>31051</v>
-      </c>
-      <c r="I8" s="115">
-        <v>12.3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="7">
-        <v>1290</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="7">
-        <v>113</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="116">
-        <v>31050</v>
-      </c>
-      <c r="I9" s="115">
-        <v>13.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="7">
-        <v>1293</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="7">
-        <v>205</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="116">
-        <v>30939</v>
-      </c>
-      <c r="I10" s="115">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="7">
-        <v>1299</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="7">
-        <v>127</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="116">
-        <v>32863</v>
-      </c>
-      <c r="I11" s="115">
-        <v>12.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="7">
-        <v>1302</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" s="7">
-        <v>139</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="116">
-        <v>30900</v>
-      </c>
-      <c r="I12" s="115">
-        <v>14.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="7">
-        <v>1310</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="7">
-        <v>137</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="116">
-        <v>31689</v>
-      </c>
-      <c r="I13" s="115">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="7">
-        <v>1329</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="7">
-        <v>151</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="116">
-        <v>32561</v>
-      </c>
-      <c r="I14" s="115">
-        <v>10.35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="7">
-        <v>1333</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="7">
-        <v>122</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" s="116">
-        <v>32979</v>
-      </c>
-      <c r="I15" s="115">
-        <v>10.15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="7">
-        <v>1368</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="7">
-        <v>132</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="116">
-        <v>30386</v>
-      </c>
-      <c r="I16" s="115">
-        <v>12.25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="7">
-        <v>1509</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F17" s="7">
-        <v>135</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17" s="116">
-        <v>31217</v>
-      </c>
-      <c r="I17" s="115">
-        <v>13.25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="7">
-        <v>1516</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="7">
-        <v>105</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="116">
-        <v>31112</v>
-      </c>
-      <c r="I18" s="115">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="7">
-        <v>1529</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" s="7">
-        <v>129</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="116">
-        <v>31805</v>
-      </c>
-      <c r="I19" s="115">
-        <v>11.3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="7">
-        <v>1656</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F20" s="7">
-        <v>149</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" s="116">
-        <v>32125</v>
-      </c>
-      <c r="I20" s="115">
-        <v>12.35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="7">
-        <v>1672</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F21" s="7">
-        <v>114</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="116">
-        <v>32979</v>
-      </c>
-      <c r="I21" s="115">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="7">
-        <v>1673</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" s="7">
-        <v>112</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H22" s="116">
-        <v>33688</v>
-      </c>
-      <c r="I22" s="115">
-        <v>11.85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="7">
-        <v>1676</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" s="7">
-        <v>115</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H23" s="116">
-        <v>29885</v>
-      </c>
-      <c r="I23" s="115">
-        <v>10.75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="7">
-        <v>1721</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F24" s="7">
-        <v>102</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H24" s="116">
-        <v>33091</v>
-      </c>
-      <c r="I24" s="115">
-        <v>9.75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="7">
-        <v>1723</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F25" s="7">
-        <v>145</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H25" s="116">
-        <v>28531</v>
-      </c>
-      <c r="I25" s="115">
-        <v>13.95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="7">
-        <v>1758</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F26" s="7">
-        <v>107</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H26" s="116">
-        <v>30028</v>
-      </c>
-      <c r="I26" s="115">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="7">
-        <v>1792</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F27" s="7">
-        <v>111</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H27" s="116">
-        <v>33231</v>
-      </c>
-      <c r="I27" s="115">
-        <v>10.3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="7">
-        <v>1814</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28" s="7">
-        <v>103</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H28" s="116">
-        <v>32571</v>
-      </c>
-      <c r="I28" s="115">
-        <v>12.25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="7">
-        <v>1908</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F29" s="7">
-        <v>152</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H29" s="116">
-        <v>30817</v>
-      </c>
-      <c r="I29" s="115">
-        <v>10.25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="7">
-        <v>1931</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F30" s="7">
-        <v>110</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H30" s="116">
-        <v>32679</v>
-      </c>
-      <c r="I30" s="115">
-        <v>9.85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="7">
-        <v>1960</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F31" s="7">
-        <v>150</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H31" s="116">
-        <v>31729</v>
-      </c>
-      <c r="I31" s="115">
-        <v>11.65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="7">
-        <v>1964</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="F32" s="7">
-        <v>108</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H32" s="116">
-        <v>33559</v>
-      </c>
-      <c r="I32" s="115">
-        <v>9.25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="7">
-        <v>1975</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F33" s="7">
-        <v>125</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H33" s="116">
-        <v>35125</v>
-      </c>
-      <c r="I33" s="115">
-        <v>9.25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="7">
-        <v>1983</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F34" s="7">
-        <v>154</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H34" s="116">
-        <v>35609</v>
-      </c>
-      <c r="I34" s="115">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="7">
-        <v>1990</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="F35" s="7">
-        <v>198</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H35" s="116">
-        <v>35840</v>
-      </c>
-      <c r="I35" s="115">
-        <v>10.95</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="7">
-        <v>1995</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F36" s="7">
-        <v>198</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H36" s="116">
-        <v>35855</v>
-      </c>
-      <c r="I36" s="115">
-        <v>11.75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="7">
-        <v>1999</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="F37" s="7">
-        <v>428</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H37" s="116">
-        <v>35981</v>
-      </c>
-      <c r="I37" s="115">
-        <v>10.15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -10404,6 +9732,1100 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr codeName="Sheet17"/>
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" style="117" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="115"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="7">
+        <v>1054</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="7">
+        <v>148</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="116">
+        <v>33344</v>
+      </c>
+      <c r="I1" s="115">
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="7">
+        <v>1056</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="7">
+        <v>121</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="116">
+        <v>29153</v>
+      </c>
+      <c r="I2" s="115">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="7">
+        <v>1067</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="7">
+        <v>123</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="116">
+        <v>32040</v>
+      </c>
+      <c r="I3" s="115">
+        <v>14.55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="7">
+        <v>1075</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="7">
+        <v>126</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="116">
+        <v>33823</v>
+      </c>
+      <c r="I4" s="115">
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="7">
+        <v>1078</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="7">
+        <v>101</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="116">
+        <v>31503</v>
+      </c>
+      <c r="I5" s="115">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="7">
+        <v>1152</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="7">
+        <v>118</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="116">
+        <v>32894</v>
+      </c>
+      <c r="I6" s="115">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="7">
+        <v>1196</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="7">
+        <v>289</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="116">
+        <v>35886</v>
+      </c>
+      <c r="I7" s="115">
+        <v>9.9499999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="7">
+        <v>1284</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="7">
+        <v>124</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="116">
+        <v>31051</v>
+      </c>
+      <c r="I8" s="115">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="7">
+        <v>1290</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="7">
+        <v>113</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="116">
+        <v>31050</v>
+      </c>
+      <c r="I9" s="115">
+        <v>13.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="7">
+        <v>1293</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="7">
+        <v>205</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="116">
+        <v>30939</v>
+      </c>
+      <c r="I10" s="115">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="7">
+        <v>1299</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="7">
+        <v>127</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="116">
+        <v>32863</v>
+      </c>
+      <c r="I11" s="115">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="7">
+        <v>1302</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="7">
+        <v>139</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="116">
+        <v>30900</v>
+      </c>
+      <c r="I12" s="115">
+        <v>14.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="7">
+        <v>1310</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="7">
+        <v>137</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="116">
+        <v>31689</v>
+      </c>
+      <c r="I13" s="115">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="7">
+        <v>1329</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="7">
+        <v>151</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="116">
+        <v>32561</v>
+      </c>
+      <c r="I14" s="115">
+        <v>10.35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="7">
+        <v>1333</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="7">
+        <v>122</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="116">
+        <v>32979</v>
+      </c>
+      <c r="I15" s="115">
+        <v>10.15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="7">
+        <v>1368</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="7">
+        <v>132</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="116">
+        <v>30386</v>
+      </c>
+      <c r="I16" s="115">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="7">
+        <v>1509</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="7">
+        <v>135</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="116">
+        <v>31217</v>
+      </c>
+      <c r="I17" s="115">
+        <v>13.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="7">
+        <v>1516</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="7">
+        <v>105</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="116">
+        <v>31112</v>
+      </c>
+      <c r="I18" s="115">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="7">
+        <v>1529</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="7">
+        <v>129</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="116">
+        <v>31805</v>
+      </c>
+      <c r="I19" s="115">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="7">
+        <v>1656</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="7">
+        <v>149</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="116">
+        <v>32125</v>
+      </c>
+      <c r="I20" s="115">
+        <v>12.35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="7">
+        <v>1672</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="7">
+        <v>114</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="116">
+        <v>32979</v>
+      </c>
+      <c r="I21" s="115">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="7">
+        <v>1673</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="7">
+        <v>112</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" s="116">
+        <v>33688</v>
+      </c>
+      <c r="I22" s="115">
+        <v>11.85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="7">
+        <v>1676</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" s="7">
+        <v>115</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="116">
+        <v>29885</v>
+      </c>
+      <c r="I23" s="115">
+        <v>10.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="7">
+        <v>1721</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="7">
+        <v>102</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="116">
+        <v>33091</v>
+      </c>
+      <c r="I24" s="115">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="7">
+        <v>1723</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25" s="7">
+        <v>145</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="116">
+        <v>28531</v>
+      </c>
+      <c r="I25" s="115">
+        <v>13.95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="7">
+        <v>1758</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" s="7">
+        <v>107</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="116">
+        <v>30028</v>
+      </c>
+      <c r="I26" s="115">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="7">
+        <v>1792</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="7">
+        <v>111</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27" s="116">
+        <v>33231</v>
+      </c>
+      <c r="I27" s="115">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="7">
+        <v>1814</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="7">
+        <v>103</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="116">
+        <v>32571</v>
+      </c>
+      <c r="I28" s="115">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="7">
+        <v>1908</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F29" s="7">
+        <v>152</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="116">
+        <v>30817</v>
+      </c>
+      <c r="I29" s="115">
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="7">
+        <v>1931</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F30" s="7">
+        <v>110</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H30" s="116">
+        <v>32679</v>
+      </c>
+      <c r="I30" s="115">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="7">
+        <v>1960</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" s="7">
+        <v>150</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H31" s="116">
+        <v>31729</v>
+      </c>
+      <c r="I31" s="115">
+        <v>11.65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="7">
+        <v>1964</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F32" s="7">
+        <v>108</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H32" s="116">
+        <v>33559</v>
+      </c>
+      <c r="I32" s="115">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="7">
+        <v>1975</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F33" s="7">
+        <v>125</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H33" s="116">
+        <v>35125</v>
+      </c>
+      <c r="I33" s="115">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="7">
+        <v>1983</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" s="7">
+        <v>154</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="116">
+        <v>35609</v>
+      </c>
+      <c r="I34" s="115">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="7">
+        <v>1990</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F35" s="7">
+        <v>198</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H35" s="116">
+        <v>35840</v>
+      </c>
+      <c r="I35" s="115">
+        <v>10.95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="7">
+        <v>1995</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F36" s="7">
+        <v>198</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H36" s="116">
+        <v>35855</v>
+      </c>
+      <c r="I36" s="115">
+        <v>11.75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="7">
+        <v>1999</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F37" s="7">
+        <v>428</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" s="116">
+        <v>35981</v>
+      </c>
+      <c r="I37" s="115">
+        <v>10.15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:I37"/>
@@ -11892,7 +12314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE727711-D0A2-4196-A6AA-50DDE55C0A6F}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -13207,8 +13629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A99380-3415-42C6-8C41-613698A280FA}">
   <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -13389,6 +13811,395 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90CB938-F6AF-4391-A249-F7B9CAEC4582}">
+  <dimension ref="B1:G18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="3.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
+    <col min="5" max="6" width="13.81640625" customWidth="1"/>
+    <col min="7" max="7" width="3.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="13" thickBot="1"/>
+    <row r="2" spans="2:7" ht="21.75" customHeight="1">
+      <c r="B2" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" s="123"/>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="10">
+        <v>1054</v>
+      </c>
+      <c r="C3" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B3,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Howard</v>
+      </c>
+      <c r="D3" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B3,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Smith</v>
+      </c>
+      <c r="E3" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B3,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>AT</v>
+      </c>
+      <c r="F3" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B3,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>11.25</v>
+      </c>
+      <c r="G3" s="66"/>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="10">
+        <v>1056</v>
+      </c>
+      <c r="C4" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B4,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Joe</v>
+      </c>
+      <c r="D4" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B4,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Gonzales</v>
+      </c>
+      <c r="E4" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B4,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>AT</v>
+      </c>
+      <c r="F4" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B4,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>12.25</v>
+      </c>
+      <c r="G4" s="66"/>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="10">
+        <v>1067</v>
+      </c>
+      <c r="C5" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B5,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Gail</v>
+      </c>
+      <c r="D5" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B5,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Scote</v>
+      </c>
+      <c r="E5" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B5,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>AT</v>
+      </c>
+      <c r="F5" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B5,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>14.55</v>
+      </c>
+      <c r="G5" s="66"/>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="10">
+        <v>1075</v>
+      </c>
+      <c r="C6" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B6,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Sheryl</v>
+      </c>
+      <c r="D6" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B6,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Kane</v>
+      </c>
+      <c r="E6" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B6,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>AD</v>
+      </c>
+      <c r="F6" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B6,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>11.25</v>
+      </c>
+      <c r="G6" s="66"/>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="10">
+        <v>1078</v>
+      </c>
+      <c r="C7" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B7,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Kendrick</v>
+      </c>
+      <c r="D7" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B7,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Hapsbuch</v>
+      </c>
+      <c r="E7" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B7,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>AC</v>
+      </c>
+      <c r="F7" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B7,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="G7" s="66"/>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="10">
+        <v>1152</v>
+      </c>
+      <c r="C8" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B8,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Mark</v>
+      </c>
+      <c r="D8" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B8,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Henders</v>
+      </c>
+      <c r="E8" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B8,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>AD</v>
+      </c>
+      <c r="F8" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B8,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>12.25</v>
+      </c>
+      <c r="G8" s="66"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="10">
+        <v>1196</v>
+      </c>
+      <c r="C9" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B9,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Katie</v>
+      </c>
+      <c r="D9" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B9,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Atherton</v>
+      </c>
+      <c r="E9" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B9,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>HR</v>
+      </c>
+      <c r="F9" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B9,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="G9" s="66"/>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="10">
+        <v>1284</v>
+      </c>
+      <c r="C10" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B10,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Frank</v>
+      </c>
+      <c r="D10" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B10,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Bellwood</v>
+      </c>
+      <c r="E10" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B10,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>MK</v>
+      </c>
+      <c r="F10" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B10,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>12.3</v>
+      </c>
+      <c r="G10" s="66"/>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="10"/>
+      <c r="C11" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B11,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D11" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B11,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E11" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B11,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F11" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B11,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G11" s="66"/>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="10"/>
+      <c r="C12" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B12,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D12" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B12,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E12" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B12,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F12" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B12,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G12" s="66"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B13,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D13" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B13,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E13" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B13,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F13" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B13,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G13" s="66"/>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="10">
+        <v>1302</v>
+      </c>
+      <c r="C14" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B14,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Randy</v>
+      </c>
+      <c r="D14" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B14,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Sindole</v>
+      </c>
+      <c r="E14" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B14,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>MK</v>
+      </c>
+      <c r="F14" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B14,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>14.25</v>
+      </c>
+      <c r="G14" s="66"/>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="10">
+        <v>1310</v>
+      </c>
+      <c r="C15" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B15,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Ellen</v>
+      </c>
+      <c r="D15" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B15,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Smith</v>
+      </c>
+      <c r="E15" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B15,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>MF</v>
+      </c>
+      <c r="F15" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B15,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>11.5</v>
+      </c>
+      <c r="G15" s="66"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="10">
+        <v>1329</v>
+      </c>
+      <c r="C16" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B16,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Tuome</v>
+      </c>
+      <c r="D16" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B16,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Vuanuo</v>
+      </c>
+      <c r="E16" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B16,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>AC</v>
+      </c>
+      <c r="F16" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B16,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>10.35</v>
+      </c>
+      <c r="G16" s="66"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="10">
+        <v>1333</v>
+      </c>
+      <c r="C17" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B17,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Tadeuz</v>
+      </c>
+      <c r="D17" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B17,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Szcznyck</v>
+      </c>
+      <c r="E17" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B17,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>HR</v>
+      </c>
+      <c r="F17" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B17,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>10.15</v>
+      </c>
+      <c r="G17" s="66"/>
+    </row>
+    <row r="18" spans="2:7" ht="13" thickBot="1">
+      <c r="B18" s="13">
+        <v>1368</v>
+      </c>
+      <c r="C18" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B18,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Tammy</v>
+      </c>
+      <c r="D18" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B18,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>Wu</v>
+      </c>
+      <c r="E18" s="11" t="str">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B18,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>AD</v>
+      </c>
+      <c r="F18" s="11">
+        <f>INDEX('Master Emp List'!$A$1:$I$38,MATCH($B18,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>12.25</v>
+      </c>
+      <c r="G18" s="66"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:I38"/>
@@ -14511,425 +15322,4 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr codeName="Sheet9"/>
-  <dimension ref="A2:H26"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
-  <cols>
-    <col min="1" max="1" width="14.453125" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="3.1796875" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:8" ht="13">
-      <c r="A2" s="35" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>179</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>203</v>
-      </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="38" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" s="38" t="s">
-        <v>220</v>
-      </c>
-      <c r="G2" s="38" t="s">
-        <v>219</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="13">
-      <c r="A3" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="C3" s="24">
-        <v>13.65</v>
-      </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="17" t="str">
-        <f>LEFT(A3,3)</f>
-        <v>ACM</v>
-      </c>
-      <c r="F3" s="17" t="str">
-        <f>MID(A3,4,3)</f>
-        <v>110</v>
-      </c>
-      <c r="G3" s="17" t="str">
-        <f>RIGHT(A3,2)</f>
-        <v>WW</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="13">
-      <c r="A4" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="C4" s="24">
-        <v>12.19</v>
-      </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-    </row>
-    <row r="5" spans="1:8" ht="13">
-      <c r="A5" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C5" s="24">
-        <v>10.89</v>
-      </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-    </row>
-    <row r="6" spans="1:8" ht="13">
-      <c r="A6" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="C6" s="24">
-        <v>9.75</v>
-      </c>
-      <c r="D6" s="37"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="1:8" ht="13">
-      <c r="A7" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="C7" s="24">
-        <v>9.59</v>
-      </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-    </row>
-    <row r="8" spans="1:8" ht="13">
-      <c r="A8" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="C8" s="24">
-        <v>10.4</v>
-      </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="1:8" ht="13">
-      <c r="A9" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="C9" s="24">
-        <v>10.56</v>
-      </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-    </row>
-    <row r="10" spans="1:8" ht="13">
-      <c r="A10" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="C10" s="24">
-        <v>9.75</v>
-      </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-    </row>
-    <row r="11" spans="1:8" ht="13">
-      <c r="A11" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="C11" s="24">
-        <v>9.75</v>
-      </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-    </row>
-    <row r="12" spans="1:8" ht="13">
-      <c r="A12" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="C12" s="24">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-    </row>
-    <row r="13" spans="1:8" ht="13">
-      <c r="A13" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="C13" s="24">
-        <v>5.04</v>
-      </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-    </row>
-    <row r="14" spans="1:8" ht="13">
-      <c r="A14" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="C14" s="24">
-        <v>3.9</v>
-      </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-    </row>
-    <row r="15" spans="1:8" ht="13">
-      <c r="A15" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="C15" s="24">
-        <v>4.55</v>
-      </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16" spans="1:8" ht="13">
-      <c r="A16" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="C16" s="24">
-        <v>5.2</v>
-      </c>
-      <c r="D16" s="37"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-    </row>
-    <row r="17" spans="1:7" ht="13">
-      <c r="A17" s="22" t="s">
-        <v>209</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="C17" s="24">
-        <v>7.31</v>
-      </c>
-      <c r="D17" s="37"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-    </row>
-    <row r="18" spans="1:7" ht="13">
-      <c r="A18" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="C18" s="24">
-        <v>6.5</v>
-      </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-    </row>
-    <row r="19" spans="1:7" ht="13">
-      <c r="A19" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="C19" s="24">
-        <v>4.55</v>
-      </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-    </row>
-    <row r="20" spans="1:7" ht="13">
-      <c r="A20" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="C20" s="24">
-        <v>14.3</v>
-      </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-    </row>
-    <row r="21" spans="1:7" ht="13">
-      <c r="A21" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="C21" s="24">
-        <v>13.81</v>
-      </c>
-      <c r="D21" s="37"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-    </row>
-    <row r="22" spans="1:7" ht="13">
-      <c r="A22" s="22" t="s">
-        <v>217</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="C22" s="24">
-        <v>7.31</v>
-      </c>
-      <c r="D22" s="37"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-    </row>
-    <row r="23" spans="1:7" ht="13">
-      <c r="A23" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="C23" s="24">
-        <v>7.31</v>
-      </c>
-      <c r="D23" s="37"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-    </row>
-    <row r="24" spans="1:7" ht="13">
-      <c r="A24" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>200</v>
-      </c>
-      <c r="C24" s="24">
-        <v>7.31</v>
-      </c>
-      <c r="D24" s="37"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-    </row>
-    <row r="25" spans="1:7" ht="13">
-      <c r="A25" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="C25" s="24">
-        <v>7.64</v>
-      </c>
-      <c r="D25" s="37"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-    </row>
-    <row r="26" spans="1:7" ht="13">
-      <c r="A26" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="C26" s="24">
-        <v>6.14</v>
-      </c>
-      <c r="D26" s="37"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="0" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Creating a Dynamic HLOOKUP() with the MATCH() Function
</commit_message>
<xml_diff>
--- a/25 - Lookup Functions/Excel103-AdvancedExercises.xlsx
+++ b/25 - Lookup Functions/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/25 - Lookup Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1528" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{098BF6BF-C4AD-4715-AFE8-2D5B161880B1}"/>
+  <xr:revisionPtr revIDLastSave="1534" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0BDC9CA-74D3-40E7-B32C-A87B059707A1}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -18,86 +18,87 @@
     <sheet name="VLOOKUP Function" sheetId="1" r:id="rId3"/>
     <sheet name="Master Emp List" sheetId="35" r:id="rId4"/>
     <sheet name="HLOOKUP Function" sheetId="22" r:id="rId5"/>
-    <sheet name="Master Inventory List" sheetId="23" r:id="rId6"/>
-    <sheet name="INDEX MATCH Functions" sheetId="34" r:id="rId7"/>
-    <sheet name="INDEX MATCH Functions 2" sheetId="36" r:id="rId8"/>
-    <sheet name="INDEX MATCH Master Emp List" sheetId="5" r:id="rId9"/>
-    <sheet name="LEFT RIGHT MID Functions" sheetId="21" r:id="rId10"/>
-    <sheet name="SEARCH Function" sheetId="24" r:id="rId11"/>
-    <sheet name="CONCATENATE" sheetId="20" r:id="rId12"/>
-    <sheet name="Formula Auditing" sheetId="25" r:id="rId13"/>
-    <sheet name="Watch Window" sheetId="27" r:id="rId14"/>
-    <sheet name="Worksheet Protection" sheetId="26" r:id="rId15"/>
-    <sheet name="Goal Seek" sheetId="31" r:id="rId16"/>
-    <sheet name="Solver" sheetId="30" r:id="rId17"/>
-    <sheet name="Data Table" sheetId="28" r:id="rId18"/>
-    <sheet name="Scenarios" sheetId="29" r:id="rId19"/>
-    <sheet name="Macro" sheetId="32" r:id="rId20"/>
-    <sheet name="Test Macro" sheetId="33" r:id="rId21"/>
+    <sheet name="HLOOKUP Function 2" sheetId="37" r:id="rId6"/>
+    <sheet name="Master Inventory List" sheetId="23" r:id="rId7"/>
+    <sheet name="INDEX MATCH Functions" sheetId="34" r:id="rId8"/>
+    <sheet name="INDEX MATCH Functions 2" sheetId="36" r:id="rId9"/>
+    <sheet name="INDEX MATCH Master Emp List" sheetId="5" r:id="rId10"/>
+    <sheet name="LEFT RIGHT MID Functions" sheetId="21" r:id="rId11"/>
+    <sheet name="SEARCH Function" sheetId="24" r:id="rId12"/>
+    <sheet name="CONCATENATE" sheetId="20" r:id="rId13"/>
+    <sheet name="Formula Auditing" sheetId="25" r:id="rId14"/>
+    <sheet name="Watch Window" sheetId="27" r:id="rId15"/>
+    <sheet name="Worksheet Protection" sheetId="26" r:id="rId16"/>
+    <sheet name="Goal Seek" sheetId="31" r:id="rId17"/>
+    <sheet name="Solver" sheetId="30" r:id="rId18"/>
+    <sheet name="Data Table" sheetId="28" r:id="rId19"/>
+    <sheet name="Scenarios" sheetId="29" r:id="rId20"/>
+    <sheet name="Macro" sheetId="32" r:id="rId21"/>
+    <sheet name="Test Macro" sheetId="33" r:id="rId22"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'INDEX MATCH Master Emp List'!$A$1:$I$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'INDEX MATCH Master Emp List'!$A$1:$I$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Master Emp List'!$B$1:$I$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SUMIF Function'!$A$2:$E$272</definedName>
     <definedName name="Monthly_Goal">'IF Function'!$I$2</definedName>
-    <definedName name="solver_cvg" localSheetId="16" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="16" hidden="1">1</definedName>
+    <definedName name="solver_cvg" localSheetId="17" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="17" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="16" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="16" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="16" hidden="1">100</definedName>
-    <definedName name="solver_lhs1" localSheetId="16" hidden="1">Solver!$B$8:$E$8</definedName>
-    <definedName name="solver_lhs2" localSheetId="16" hidden="1">Solver!$B$8:$E$8</definedName>
-    <definedName name="solver_lhs3" localSheetId="16" hidden="1">Solver!$B$8:$E$8</definedName>
-    <definedName name="solver_lhs4" localSheetId="16" hidden="1">Solver!$B$8:$E$8</definedName>
-    <definedName name="solver_lhs5" localSheetId="16" hidden="1">Solver!$B$8:$E$8</definedName>
-    <definedName name="solver_lhs6" localSheetId="16" hidden="1">Solver!$E$8</definedName>
-    <definedName name="solver_lhs7" localSheetId="16" hidden="1">Solver!$E$8</definedName>
-    <definedName name="solver_lhs8" localSheetId="16" hidden="1">Solver!$E$8</definedName>
-    <definedName name="solver_lin" localSheetId="16" hidden="1">0</definedName>
-    <definedName name="solver_mip" localSheetId="16" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="16" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="16" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="16" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="17" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="17" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="17" hidden="1">100</definedName>
+    <definedName name="solver_lhs1" localSheetId="17" hidden="1">Solver!$B$8:$E$8</definedName>
+    <definedName name="solver_lhs2" localSheetId="17" hidden="1">Solver!$B$8:$E$8</definedName>
+    <definedName name="solver_lhs3" localSheetId="17" hidden="1">Solver!$B$8:$E$8</definedName>
+    <definedName name="solver_lhs4" localSheetId="17" hidden="1">Solver!$B$8:$E$8</definedName>
+    <definedName name="solver_lhs5" localSheetId="17" hidden="1">Solver!$B$8:$E$8</definedName>
+    <definedName name="solver_lhs6" localSheetId="17" hidden="1">Solver!$E$8</definedName>
+    <definedName name="solver_lhs7" localSheetId="17" hidden="1">Solver!$E$8</definedName>
+    <definedName name="solver_lhs8" localSheetId="17" hidden="1">Solver!$E$8</definedName>
+    <definedName name="solver_lin" localSheetId="17" hidden="1">0</definedName>
+    <definedName name="solver_mip" localSheetId="17" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="17" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="17" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="17" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="16" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="16" hidden="1">2147483647</definedName>
+    <definedName name="solver_neg" localSheetId="17" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="17" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="16" hidden="1">0</definedName>
-    <definedName name="solver_nwt" localSheetId="16" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="17" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="17" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'IF Function'!$I$2</definedName>
-    <definedName name="solver_opt" localSheetId="16" hidden="1">Solver!$H$8</definedName>
-    <definedName name="solver_pre" localSheetId="16" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="16" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="16" hidden="1">2</definedName>
-    <definedName name="solver_rel2" localSheetId="16" hidden="1">2</definedName>
-    <definedName name="solver_rel3" localSheetId="16" hidden="1">2</definedName>
-    <definedName name="solver_rel4" localSheetId="16" hidden="1">2</definedName>
-    <definedName name="solver_rel5" localSheetId="16" hidden="1">2</definedName>
-    <definedName name="solver_rel6" localSheetId="16" hidden="1">2</definedName>
-    <definedName name="solver_rel7" localSheetId="16" hidden="1">2</definedName>
-    <definedName name="solver_rel8" localSheetId="16" hidden="1">2</definedName>
-    <definedName name="solver_rhs1" localSheetId="16" hidden="1">Solver!$B$10:$E$10</definedName>
-    <definedName name="solver_rhs2" localSheetId="16" hidden="1">Solver!$B$10:$E$10</definedName>
-    <definedName name="solver_rhs3" localSheetId="16" hidden="1">Solver!$B$10:$E$10</definedName>
-    <definedName name="solver_rhs4" localSheetId="16" hidden="1">Solver!$B$10:$E$10</definedName>
-    <definedName name="solver_rhs5" localSheetId="16" hidden="1">Solver!$B$10:$E$10</definedName>
-    <definedName name="solver_rhs6" localSheetId="16" hidden="1">Solver!$E$10</definedName>
-    <definedName name="solver_rhs7" localSheetId="16" hidden="1">Solver!$E$10</definedName>
-    <definedName name="solver_rhs8" localSheetId="16" hidden="1">Solver!$E$10</definedName>
-    <definedName name="solver_rlx" localSheetId="16" hidden="1">1</definedName>
-    <definedName name="solver_rsd" localSheetId="16" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="16" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="16" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="16" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="16" hidden="1">100</definedName>
-    <definedName name="solver_tol" localSheetId="16" hidden="1">0.05</definedName>
+    <definedName name="solver_opt" localSheetId="17" hidden="1">Solver!$H$8</definedName>
+    <definedName name="solver_pre" localSheetId="17" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="17" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="17" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="17" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="17" hidden="1">2</definedName>
+    <definedName name="solver_rel4" localSheetId="17" hidden="1">2</definedName>
+    <definedName name="solver_rel5" localSheetId="17" hidden="1">2</definedName>
+    <definedName name="solver_rel6" localSheetId="17" hidden="1">2</definedName>
+    <definedName name="solver_rel7" localSheetId="17" hidden="1">2</definedName>
+    <definedName name="solver_rel8" localSheetId="17" hidden="1">2</definedName>
+    <definedName name="solver_rhs1" localSheetId="17" hidden="1">Solver!$B$10:$E$10</definedName>
+    <definedName name="solver_rhs2" localSheetId="17" hidden="1">Solver!$B$10:$E$10</definedName>
+    <definedName name="solver_rhs3" localSheetId="17" hidden="1">Solver!$B$10:$E$10</definedName>
+    <definedName name="solver_rhs4" localSheetId="17" hidden="1">Solver!$B$10:$E$10</definedName>
+    <definedName name="solver_rhs5" localSheetId="17" hidden="1">Solver!$B$10:$E$10</definedName>
+    <definedName name="solver_rhs6" localSheetId="17" hidden="1">Solver!$E$10</definedName>
+    <definedName name="solver_rhs7" localSheetId="17" hidden="1">Solver!$E$10</definedName>
+    <definedName name="solver_rhs8" localSheetId="17" hidden="1">Solver!$E$10</definedName>
+    <definedName name="solver_rlx" localSheetId="17" hidden="1">1</definedName>
+    <definedName name="solver_rsd" localSheetId="17" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="17" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="17" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="17" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="17" hidden="1">100</definedName>
+    <definedName name="solver_tol" localSheetId="17" hidden="1">0.05</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="16" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="17" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="16" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="17" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="16" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="17" hidden="1">3</definedName>
     <definedName name="Totals">'IF Function'!$F$5:$F$9</definedName>
     <definedName name="Week_1">'IF Function'!$B$5:$B$9</definedName>
     <definedName name="Week_2">'IF Function'!$C$5:$C$9</definedName>
@@ -119,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="284">
   <si>
     <t>Monthly Goal:</t>
   </si>
@@ -1967,13 +1968,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2932,6 +2933,1131 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet11"/>
+  <dimension ref="A1:I38"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" customHeight="1"/>
+  <cols>
+    <col min="1" max="8" width="14.1796875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="24.75" customHeight="1">
+      <c r="A1" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A2" s="7">
+        <v>1054</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="7">
+        <v>148</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="8">
+        <v>33344</v>
+      </c>
+      <c r="I2" s="9">
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A3" s="7">
+        <v>1056</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="7">
+        <v>121</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="8">
+        <v>29153</v>
+      </c>
+      <c r="I3" s="9">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A4" s="7">
+        <v>1067</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="7">
+        <v>123</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="8">
+        <v>32040</v>
+      </c>
+      <c r="I4" s="9">
+        <v>14.55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A5" s="7">
+        <v>1075</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="7">
+        <v>126</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="8">
+        <v>33823</v>
+      </c>
+      <c r="I5" s="9">
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A6" s="7">
+        <v>1078</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="7">
+        <v>101</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="8">
+        <v>31503</v>
+      </c>
+      <c r="I6" s="9">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A7" s="7">
+        <v>1152</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="7">
+        <v>118</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="8">
+        <v>32894</v>
+      </c>
+      <c r="I7" s="9">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A8" s="7">
+        <v>1196</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="7">
+        <v>289</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="8">
+        <v>35886</v>
+      </c>
+      <c r="I8" s="9">
+        <v>9.9499999999999993</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A9" s="7">
+        <v>1284</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="7">
+        <v>124</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="8">
+        <v>31051</v>
+      </c>
+      <c r="I9" s="9">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A10" s="7">
+        <v>1290</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="7">
+        <v>113</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="8">
+        <v>31050</v>
+      </c>
+      <c r="I10" s="9">
+        <v>13.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A11" s="7">
+        <v>1293</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="7">
+        <v>205</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="8">
+        <v>30939</v>
+      </c>
+      <c r="I11" s="9">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A12" s="7">
+        <v>1299</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="7">
+        <v>127</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="8">
+        <v>32863</v>
+      </c>
+      <c r="I12" s="9">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A13" s="7">
+        <v>1302</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="7">
+        <v>139</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="8">
+        <v>30900</v>
+      </c>
+      <c r="I13" s="9">
+        <v>14.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A14" s="7">
+        <v>1310</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="7">
+        <v>137</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="8">
+        <v>31689</v>
+      </c>
+      <c r="I14" s="9">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A15" s="7">
+        <v>1329</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="7">
+        <v>151</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="8">
+        <v>32561</v>
+      </c>
+      <c r="I15" s="9">
+        <v>10.35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A16" s="7">
+        <v>1333</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="7">
+        <v>122</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="8">
+        <v>32979</v>
+      </c>
+      <c r="I16" s="9">
+        <v>10.15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A17" s="7">
+        <v>1368</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="7">
+        <v>132</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="8">
+        <v>30386</v>
+      </c>
+      <c r="I17" s="9">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A18" s="7">
+        <v>1509</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="7">
+        <v>135</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="8">
+        <v>31217</v>
+      </c>
+      <c r="I18" s="9">
+        <v>13.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A19" s="7">
+        <v>1516</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="7">
+        <v>105</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="8">
+        <v>31112</v>
+      </c>
+      <c r="I19" s="9">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A20" s="7">
+        <v>1529</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="7">
+        <v>129</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="8">
+        <v>31805</v>
+      </c>
+      <c r="I20" s="9">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A21" s="7">
+        <v>1656</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="7">
+        <v>149</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="8">
+        <v>32125</v>
+      </c>
+      <c r="I21" s="9">
+        <v>12.35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A22" s="7">
+        <v>1672</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="7">
+        <v>114</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="8">
+        <v>32979</v>
+      </c>
+      <c r="I22" s="9">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A23" s="7">
+        <v>1673</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="7">
+        <v>112</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="8">
+        <v>33688</v>
+      </c>
+      <c r="I23" s="9">
+        <v>11.85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A24" s="7">
+        <v>1676</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" s="7">
+        <v>115</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="8">
+        <v>29885</v>
+      </c>
+      <c r="I24" s="9">
+        <v>10.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A25" s="7">
+        <v>1721</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" s="7">
+        <v>102</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="8">
+        <v>33091</v>
+      </c>
+      <c r="I25" s="9">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A26" s="7">
+        <v>1723</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" s="7">
+        <v>145</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H26" s="8">
+        <v>28531</v>
+      </c>
+      <c r="I26" s="9">
+        <v>13.95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A27" s="7">
+        <v>1758</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="7">
+        <v>107</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" s="8">
+        <v>30028</v>
+      </c>
+      <c r="I27" s="9">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A28" s="7">
+        <v>1792</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28" s="7">
+        <v>111</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="8">
+        <v>33231</v>
+      </c>
+      <c r="I28" s="9">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A29" s="7">
+        <v>1814</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F29" s="7">
+        <v>103</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="8">
+        <v>32571</v>
+      </c>
+      <c r="I29" s="9">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A30" s="7">
+        <v>1908</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="7">
+        <v>152</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H30" s="8">
+        <v>30817</v>
+      </c>
+      <c r="I30" s="9">
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A31" s="7">
+        <v>1931</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F31" s="7">
+        <v>110</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H31" s="8">
+        <v>32679</v>
+      </c>
+      <c r="I31" s="9">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A32" s="7">
+        <v>1960</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F32" s="7">
+        <v>150</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H32" s="8">
+        <v>31729</v>
+      </c>
+      <c r="I32" s="9">
+        <v>11.65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A33" s="7">
+        <v>1964</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F33" s="7">
+        <v>108</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H33" s="8">
+        <v>33559</v>
+      </c>
+      <c r="I33" s="9">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A34" s="7">
+        <v>1975</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F34" s="7">
+        <v>125</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H34" s="8">
+        <v>35125</v>
+      </c>
+      <c r="I34" s="9">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A35" s="7">
+        <v>1983</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F35" s="7">
+        <v>154</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H35" s="8">
+        <v>35609</v>
+      </c>
+      <c r="I35" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A36" s="7">
+        <v>1990</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F36" s="7">
+        <v>198</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H36" s="8">
+        <v>35840</v>
+      </c>
+      <c r="I36" s="9">
+        <v>10.95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A37" s="7">
+        <v>1995</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F37" s="7">
+        <v>198</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" s="8">
+        <v>35855</v>
+      </c>
+      <c r="I37" s="9">
+        <v>11.75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A38" s="7">
+        <v>1999</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F38" s="7">
+        <v>428</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" s="8">
+        <v>35981</v>
+      </c>
+      <c r="I38" s="9">
+        <v>10.15</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A2:H26"/>
@@ -3352,7 +4478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C6"/>
@@ -3410,7 +4536,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:F18"/>
@@ -3434,10 +4560,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="E2" s="130" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="132"/>
+      <c r="F2" s="130"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -3446,11 +4572,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="130" t="str">
+      <c r="E3" s="131" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="131"/>
+      <c r="F3" s="132"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -3459,8 +4585,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="130"/>
-      <c r="F4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="132"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -3469,8 +4595,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="130"/>
-      <c r="F5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="132"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -3479,8 +4605,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="130"/>
-      <c r="F6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="132"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -3489,8 +4615,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="130"/>
-      <c r="F7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="132"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -3499,8 +4625,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="130"/>
-      <c r="F8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="132"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -3509,8 +4635,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="131"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="132"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -3519,8 +4645,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="130"/>
-      <c r="F10" s="131"/>
+      <c r="E10" s="131"/>
+      <c r="F10" s="132"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -3529,8 +4655,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="130"/>
-      <c r="F11" s="131"/>
+      <c r="E11" s="131"/>
+      <c r="F11" s="132"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -3539,8 +4665,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="130"/>
-      <c r="F12" s="131"/>
+      <c r="E12" s="131"/>
+      <c r="F12" s="132"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -3549,8 +4675,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="130"/>
-      <c r="F13" s="131"/>
+      <c r="E13" s="131"/>
+      <c r="F13" s="132"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -3559,8 +4685,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="130"/>
-      <c r="F14" s="131"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="132"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -3569,8 +4695,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="130"/>
-      <c r="F15" s="131"/>
+      <c r="E15" s="131"/>
+      <c r="F15" s="132"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -3579,8 +4705,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="130"/>
-      <c r="F16" s="131"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="132"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -3589,8 +4715,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="130"/>
-      <c r="F17" s="131"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="132"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -3599,11 +4725,18 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="130"/>
-      <c r="F18" s="131"/>
+      <c r="E18" s="131"/>
+      <c r="F18" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3614,13 +4747,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3628,7 +4754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:I14"/>
@@ -3901,7 +5027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:B2"/>
@@ -3930,7 +5056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:I14"/>
@@ -4204,7 +5330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:D4"/>
@@ -4258,7 +5384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:H11"/>
@@ -4466,7 +5592,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="B2:C14"/>
@@ -4566,217 +5692,6 @@
   <printOptions gridLines="1" gridLinesSet="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;A</oddHeader>
-    <oddFooter>Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr codeName="Sheet16"/>
-  <dimension ref="B2:G14"/>
-  <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
-  <cols>
-    <col min="1" max="1" width="9.1796875" style="73"/>
-    <col min="2" max="2" width="11.54296875" style="73" customWidth="1"/>
-    <col min="3" max="6" width="14.81640625" style="73" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" style="73" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="73"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:7" ht="15.5">
-      <c r="B2" s="110" t="s">
-        <v>266</v>
-      </c>
-      <c r="C2" s="110" t="s">
-        <v>265</v>
-      </c>
-      <c r="D2" s="110" t="s">
-        <v>264</v>
-      </c>
-      <c r="E2" s="110" t="s">
-        <v>263</v>
-      </c>
-      <c r="F2" s="110" t="s">
-        <v>262</v>
-      </c>
-      <c r="G2" s="110" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="13">
-      <c r="B3" s="111" t="s">
-        <v>258</v>
-      </c>
-      <c r="C3" s="112">
-        <v>85292.25</v>
-      </c>
-      <c r="D3" s="112">
-        <f>C3*C11+C3</f>
-        <v>88106.894249999998</v>
-      </c>
-      <c r="E3" s="112">
-        <f>D3*C11+D3</f>
-        <v>91014.421760249999</v>
-      </c>
-      <c r="F3" s="112">
-        <f>E3*C11+E3</f>
-        <v>94017.897678338253</v>
-      </c>
-      <c r="G3" s="112">
-        <f>SUM(C3:F3)</f>
-        <v>358431.46368858824</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="13">
-      <c r="B4" s="111" t="s">
-        <v>257</v>
-      </c>
-      <c r="C4" s="112">
-        <v>75891.25</v>
-      </c>
-      <c r="D4" s="112">
-        <f>C4*C12+C4</f>
-        <v>77636.748749999999</v>
-      </c>
-      <c r="E4" s="112">
-        <f>D4*C12+D4</f>
-        <v>79422.39397125</v>
-      </c>
-      <c r="F4" s="112">
-        <f>E4*C12+E4</f>
-        <v>81249.109032588749</v>
-      </c>
-      <c r="G4" s="112">
-        <f>SUM(C4:F4)</f>
-        <v>314199.50175383873</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="13">
-      <c r="B5" s="111" t="s">
-        <v>256</v>
-      </c>
-      <c r="C5" s="112">
-        <v>90568.34</v>
-      </c>
-      <c r="D5" s="112">
-        <f>C5*C13+C5</f>
-        <v>94462.778619999997</v>
-      </c>
-      <c r="E5" s="112">
-        <f>D5*C13+D5</f>
-        <v>98524.678100659992</v>
-      </c>
-      <c r="F5" s="112">
-        <f>E5*C13+E5</f>
-        <v>102761.23925898837</v>
-      </c>
-      <c r="G5" s="112">
-        <f>SUM(C5:F5)</f>
-        <v>386317.03597964835</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="13">
-      <c r="B6" s="111" t="s">
-        <v>255</v>
-      </c>
-      <c r="C6" s="112">
-        <v>65897.25</v>
-      </c>
-      <c r="D6" s="112">
-        <f>C6*C14+C6</f>
-        <v>66622.119749999998</v>
-      </c>
-      <c r="E6" s="112">
-        <f>D6*C14+D6</f>
-        <v>67354.963067249992</v>
-      </c>
-      <c r="F6" s="112">
-        <f>E6*C14+E6</f>
-        <v>68095.867660989737</v>
-      </c>
-      <c r="G6" s="112">
-        <f>SUM(C6:F6)</f>
-        <v>267970.20047823974</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="15.5">
-      <c r="B7" s="99" t="s">
-        <v>260</v>
-      </c>
-      <c r="C7" s="76">
-        <f>SUM(C3:C6)</f>
-        <v>317649.08999999997</v>
-      </c>
-      <c r="D7" s="76">
-        <f>SUM(D3:D6)</f>
-        <v>326828.54136999999</v>
-      </c>
-      <c r="E7" s="76">
-        <f>SUM(E3:E6)</f>
-        <v>336316.45689940994</v>
-      </c>
-      <c r="F7" s="76">
-        <f>SUM(F3:F6)</f>
-        <v>346124.11363090511</v>
-      </c>
-      <c r="G7" s="76">
-        <f>SUM(G3:G6)</f>
-        <v>1326918.201900315</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="13">
-      <c r="B10" s="133" t="s">
-        <v>259</v>
-      </c>
-      <c r="C10" s="133"/>
-    </row>
-    <row r="11" spans="2:7" ht="13">
-      <c r="B11" s="113" t="s">
-        <v>258</v>
-      </c>
-      <c r="C11" s="114">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="13">
-      <c r="B12" s="113" t="s">
-        <v>257</v>
-      </c>
-      <c r="C12" s="114">
-        <v>2.3E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="13">
-      <c r="B13" s="113" t="s">
-        <v>256</v>
-      </c>
-      <c r="C13" s="114">
-        <v>4.2999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="13">
-      <c r="B14" s="113" t="s">
-        <v>255</v>
-      </c>
-      <c r="C14" s="114">
-        <v>1.0999999999999999E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B10:C10"/>
-  </mergeCells>
-  <printOptions gridLines="1" gridLinesSet="0"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;A</oddHeader>
     <oddFooter>Page &amp;P</oddFooter>
@@ -9732,6 +10647,217 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr codeName="Sheet16"/>
+  <dimension ref="B2:G14"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="9.1796875" style="73"/>
+    <col min="2" max="2" width="11.54296875" style="73" customWidth="1"/>
+    <col min="3" max="6" width="14.81640625" style="73" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" style="73" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="73"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="15.5">
+      <c r="B2" s="110" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" s="110" t="s">
+        <v>265</v>
+      </c>
+      <c r="D2" s="110" t="s">
+        <v>264</v>
+      </c>
+      <c r="E2" s="110" t="s">
+        <v>263</v>
+      </c>
+      <c r="F2" s="110" t="s">
+        <v>262</v>
+      </c>
+      <c r="G2" s="110" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="13">
+      <c r="B3" s="111" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="112">
+        <v>85292.25</v>
+      </c>
+      <c r="D3" s="112">
+        <f>C3*C11+C3</f>
+        <v>88106.894249999998</v>
+      </c>
+      <c r="E3" s="112">
+        <f>D3*C11+D3</f>
+        <v>91014.421760249999</v>
+      </c>
+      <c r="F3" s="112">
+        <f>E3*C11+E3</f>
+        <v>94017.897678338253</v>
+      </c>
+      <c r="G3" s="112">
+        <f>SUM(C3:F3)</f>
+        <v>358431.46368858824</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="13">
+      <c r="B4" s="111" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="112">
+        <v>75891.25</v>
+      </c>
+      <c r="D4" s="112">
+        <f>C4*C12+C4</f>
+        <v>77636.748749999999</v>
+      </c>
+      <c r="E4" s="112">
+        <f>D4*C12+D4</f>
+        <v>79422.39397125</v>
+      </c>
+      <c r="F4" s="112">
+        <f>E4*C12+E4</f>
+        <v>81249.109032588749</v>
+      </c>
+      <c r="G4" s="112">
+        <f>SUM(C4:F4)</f>
+        <v>314199.50175383873</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="13">
+      <c r="B5" s="111" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5" s="112">
+        <v>90568.34</v>
+      </c>
+      <c r="D5" s="112">
+        <f>C5*C13+C5</f>
+        <v>94462.778619999997</v>
+      </c>
+      <c r="E5" s="112">
+        <f>D5*C13+D5</f>
+        <v>98524.678100659992</v>
+      </c>
+      <c r="F5" s="112">
+        <f>E5*C13+E5</f>
+        <v>102761.23925898837</v>
+      </c>
+      <c r="G5" s="112">
+        <f>SUM(C5:F5)</f>
+        <v>386317.03597964835</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="13">
+      <c r="B6" s="111" t="s">
+        <v>255</v>
+      </c>
+      <c r="C6" s="112">
+        <v>65897.25</v>
+      </c>
+      <c r="D6" s="112">
+        <f>C6*C14+C6</f>
+        <v>66622.119749999998</v>
+      </c>
+      <c r="E6" s="112">
+        <f>D6*C14+D6</f>
+        <v>67354.963067249992</v>
+      </c>
+      <c r="F6" s="112">
+        <f>E6*C14+E6</f>
+        <v>68095.867660989737</v>
+      </c>
+      <c r="G6" s="112">
+        <f>SUM(C6:F6)</f>
+        <v>267970.20047823974</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15.5">
+      <c r="B7" s="99" t="s">
+        <v>260</v>
+      </c>
+      <c r="C7" s="76">
+        <f>SUM(C3:C6)</f>
+        <v>317649.08999999997</v>
+      </c>
+      <c r="D7" s="76">
+        <f>SUM(D3:D6)</f>
+        <v>326828.54136999999</v>
+      </c>
+      <c r="E7" s="76">
+        <f>SUM(E3:E6)</f>
+        <v>336316.45689940994</v>
+      </c>
+      <c r="F7" s="76">
+        <f>SUM(F3:F6)</f>
+        <v>346124.11363090511</v>
+      </c>
+      <c r="G7" s="76">
+        <f>SUM(G3:G6)</f>
+        <v>1326918.201900315</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="13">
+      <c r="B10" s="133" t="s">
+        <v>259</v>
+      </c>
+      <c r="C10" s="133"/>
+    </row>
+    <row r="11" spans="2:7" ht="13">
+      <c r="B11" s="113" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" s="114">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="13">
+      <c r="B12" s="113" t="s">
+        <v>257</v>
+      </c>
+      <c r="C12" s="114">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="13">
+      <c r="B13" s="113" t="s">
+        <v>256</v>
+      </c>
+      <c r="C13" s="114">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="13">
+      <c r="B14" s="113" t="s">
+        <v>255</v>
+      </c>
+      <c r="C14" s="114">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B10:C10"/>
+  </mergeCells>
+  <printOptions gridLines="1" gridLinesSet="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;A</oddHeader>
+    <oddFooter>Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:I37"/>
@@ -10825,7 +11951,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:I37"/>
@@ -13441,8 +14567,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
@@ -13513,6 +14639,81 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F7437D-A8FC-427C-8A49-940F6F4A8FBE}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="30.1796875" style="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" style="54" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" style="54" customWidth="1"/>
+    <col min="4" max="4" width="8.1796875" style="54" customWidth="1"/>
+    <col min="5" max="5" width="7.26953125" style="54" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" style="54" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" style="54" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="54"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13" thickBot="1"/>
+    <row r="2" spans="1:2" ht="22.5" customHeight="1" thickBot="1">
+      <c r="A2" s="128" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="129"/>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A3" s="60" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="7.5" customHeight="1" thickTop="1">
+      <c r="A4" s="58"/>
+      <c r="B4" s="57"/>
+    </row>
+    <row r="5" spans="1:2" ht="13">
+      <c r="A5" s="61" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5" s="56">
+        <f>HLOOKUP($B$3,'Master Inventory List'!$A$2:$G$5,MATCH(LEFT(A5,11),'Master Inventory List'!$A$2:$A$5,0),FALSE)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="13">
+      <c r="A6" s="61" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" s="56">
+        <f>HLOOKUP($B$3,'Master Inventory List'!$A$2:$G$5,MATCH(LEFT(A6,11),'Master Inventory List'!$A$2:$A$5,0),FALSE)</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="13.5" thickBot="1">
+      <c r="A7" s="62" t="s">
+        <v>227</v>
+      </c>
+      <c r="B7" s="56">
+        <f>HLOOKUP($B$3,'Master Inventory List'!$A$2:$G$5,MATCH(LEFT(A7,11),'Master Inventory List'!$A$2:$A$5,0),FALSE)</f>
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:G5"/>
@@ -13625,7 +14826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A99380-3415-42C6-8C41-613698A280FA}">
   <dimension ref="B2:F19"/>
   <sheetViews>
@@ -13810,12 +15011,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90CB938-F6AF-4391-A249-F7B9CAEC4582}">
   <dimension ref="B1:G18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -14197,1129 +15398,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:I38"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" customHeight="1"/>
-  <cols>
-    <col min="1" max="8" width="14.1796875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A1" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="32" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A2" s="7">
-        <v>1054</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="7">
-        <v>148</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="8">
-        <v>33344</v>
-      </c>
-      <c r="I2" s="9">
-        <v>11.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A3" s="7">
-        <v>1056</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="7">
-        <v>121</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="8">
-        <v>29153</v>
-      </c>
-      <c r="I3" s="9">
-        <v>12.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A4" s="7">
-        <v>1067</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="7">
-        <v>123</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="8">
-        <v>32040</v>
-      </c>
-      <c r="I4" s="9">
-        <v>14.55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A5" s="7">
-        <v>1075</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="7">
-        <v>126</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="8">
-        <v>33823</v>
-      </c>
-      <c r="I5" s="9">
-        <v>11.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A6" s="7">
-        <v>1078</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="7">
-        <v>101</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="8">
-        <v>31503</v>
-      </c>
-      <c r="I6" s="9">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A7" s="7">
-        <v>1152</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="7">
-        <v>118</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="8">
-        <v>32894</v>
-      </c>
-      <c r="I7" s="9">
-        <v>12.25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A8" s="7">
-        <v>1196</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="7">
-        <v>289</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="8">
-        <v>35886</v>
-      </c>
-      <c r="I8" s="9">
-        <v>9.9499999999999993</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A9" s="7">
-        <v>1284</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="7">
-        <v>124</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="8">
-        <v>31051</v>
-      </c>
-      <c r="I9" s="9">
-        <v>12.3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A10" s="7">
-        <v>1290</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="7">
-        <v>113</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="8">
-        <v>31050</v>
-      </c>
-      <c r="I10" s="9">
-        <v>13.25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A11" s="7">
-        <v>1293</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="7">
-        <v>205</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="8">
-        <v>30939</v>
-      </c>
-      <c r="I11" s="9">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A12" s="7">
-        <v>1299</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="7">
-        <v>127</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="8">
-        <v>32863</v>
-      </c>
-      <c r="I12" s="9">
-        <v>12.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A13" s="7">
-        <v>1302</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="7">
-        <v>139</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="8">
-        <v>30900</v>
-      </c>
-      <c r="I13" s="9">
-        <v>14.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A14" s="7">
-        <v>1310</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" s="7">
-        <v>137</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" s="8">
-        <v>31689</v>
-      </c>
-      <c r="I14" s="9">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A15" s="7">
-        <v>1329</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="7">
-        <v>151</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="8">
-        <v>32561</v>
-      </c>
-      <c r="I15" s="9">
-        <v>10.35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A16" s="7">
-        <v>1333</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="7">
-        <v>122</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H16" s="8">
-        <v>32979</v>
-      </c>
-      <c r="I16" s="9">
-        <v>10.15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A17" s="7">
-        <v>1368</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" s="7">
-        <v>132</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="8">
-        <v>30386</v>
-      </c>
-      <c r="I17" s="9">
-        <v>12.25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A18" s="7">
-        <v>1509</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F18" s="7">
-        <v>135</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" s="8">
-        <v>31217</v>
-      </c>
-      <c r="I18" s="9">
-        <v>13.25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A19" s="7">
-        <v>1516</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F19" s="7">
-        <v>105</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="8">
-        <v>31112</v>
-      </c>
-      <c r="I19" s="9">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A20" s="7">
-        <v>1529</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20" s="7">
-        <v>129</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" s="8">
-        <v>31805</v>
-      </c>
-      <c r="I20" s="9">
-        <v>11.3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A21" s="7">
-        <v>1656</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" s="7">
-        <v>149</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="8">
-        <v>32125</v>
-      </c>
-      <c r="I21" s="9">
-        <v>12.35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A22" s="7">
-        <v>1672</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F22" s="7">
-        <v>114</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="8">
-        <v>32979</v>
-      </c>
-      <c r="I22" s="9">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A23" s="7">
-        <v>1673</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F23" s="7">
-        <v>112</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H23" s="8">
-        <v>33688</v>
-      </c>
-      <c r="I23" s="9">
-        <v>11.85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A24" s="7">
-        <v>1676</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F24" s="7">
-        <v>115</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H24" s="8">
-        <v>29885</v>
-      </c>
-      <c r="I24" s="9">
-        <v>10.75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A25" s="7">
-        <v>1721</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F25" s="7">
-        <v>102</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H25" s="8">
-        <v>33091</v>
-      </c>
-      <c r="I25" s="9">
-        <v>9.75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A26" s="7">
-        <v>1723</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F26" s="7">
-        <v>145</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H26" s="8">
-        <v>28531</v>
-      </c>
-      <c r="I26" s="9">
-        <v>13.95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A27" s="7">
-        <v>1758</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F27" s="7">
-        <v>107</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H27" s="8">
-        <v>30028</v>
-      </c>
-      <c r="I27" s="9">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A28" s="7">
-        <v>1792</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F28" s="7">
-        <v>111</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H28" s="8">
-        <v>33231</v>
-      </c>
-      <c r="I28" s="9">
-        <v>10.3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A29" s="7">
-        <v>1814</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F29" s="7">
-        <v>103</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H29" s="8">
-        <v>32571</v>
-      </c>
-      <c r="I29" s="9">
-        <v>12.25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A30" s="7">
-        <v>1908</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F30" s="7">
-        <v>152</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H30" s="8">
-        <v>30817</v>
-      </c>
-      <c r="I30" s="9">
-        <v>10.25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A31" s="7">
-        <v>1931</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F31" s="7">
-        <v>110</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H31" s="8">
-        <v>32679</v>
-      </c>
-      <c r="I31" s="9">
-        <v>9.85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A32" s="7">
-        <v>1960</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F32" s="7">
-        <v>150</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H32" s="8">
-        <v>31729</v>
-      </c>
-      <c r="I32" s="9">
-        <v>11.65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A33" s="7">
-        <v>1964</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="F33" s="7">
-        <v>108</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H33" s="8">
-        <v>33559</v>
-      </c>
-      <c r="I33" s="9">
-        <v>9.25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A34" s="7">
-        <v>1975</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F34" s="7">
-        <v>125</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H34" s="8">
-        <v>35125</v>
-      </c>
-      <c r="I34" s="9">
-        <v>9.25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A35" s="7">
-        <v>1983</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F35" s="7">
-        <v>154</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H35" s="8">
-        <v>35609</v>
-      </c>
-      <c r="I35" s="9">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A36" s="7">
-        <v>1990</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="F36" s="7">
-        <v>198</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H36" s="8">
-        <v>35840</v>
-      </c>
-      <c r="I36" s="9">
-        <v>10.95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A37" s="7">
-        <v>1995</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F37" s="7">
-        <v>198</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H37" s="8">
-        <v>35855</v>
-      </c>
-      <c r="I37" s="9">
-        <v>11.75</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A38" s="7">
-        <v>1999</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="F38" s="7">
-        <v>428</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H38" s="8">
-        <v>35981</v>
-      </c>
-      <c r="I38" s="9">
-        <v>10.15</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="0" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
 </file>
</xml_diff>